<commit_message>
Changes to weibull curve instead of sigmoidal curve for clean dispatchable requirement due to calculation issues.
</commit_message>
<xml_diff>
--- a/InputData/elec/CDRDfRCP/Cln Dsptchble Rsrc Dmnd for Rlbty Curve Param.xlsx
+++ b/InputData/elec/CDRDfRCP/Cln Dsptchble Rsrc Dmnd for Rlbty Curve Param.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\CDRDfRCP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C0A9FB-66F9-47E6-BEC9-2D0B0D7D12BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C7436E-9A4F-462D-A67B-5497D9E3A17C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8520" yWindow="2740" windowWidth="28800" windowHeight="15540" activeTab="1" xr2:uid="{DDCF7A3C-4581-48BB-A680-D5CBB461C8EB}"/>
+    <workbookView xWindow="4815" yWindow="1995" windowWidth="27360" windowHeight="16410" xr2:uid="{DDCF7A3C-4581-48BB-A680-D5CBB461C8EB}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -426,16 +426,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B207133-CFE8-4DB4-95CD-9BA248AF1C6C}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -443,12 +443,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -456,7 +456,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -473,32 +473,32 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1">
-        <v>-11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Set clean firm requirement for CES to 0
</commit_message>
<xml_diff>
--- a/InputData/elec/CDRDfRCP/Cln Dsptchble Rsrc Dmnd for Rlbty Curve Param.xlsx
+++ b/InputData/elec/CDRDfRCP/Cln Dsptchble Rsrc Dmnd for Rlbty Curve Param.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\CDRDfRCP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\CDRDfRCP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C7436E-9A4F-462D-A67B-5497D9E3A17C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D7C115-3F36-463E-8E5F-B756F35079A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4815" yWindow="1995" windowWidth="27360" windowHeight="16410" xr2:uid="{DDCF7A3C-4581-48BB-A680-D5CBB461C8EB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{DDCF7A3C-4581-48BB-A680-D5CBB461C8EB}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -128,9 +128,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -168,7 +168,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -274,7 +274,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -416,7 +416,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -474,7 +474,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,7 +503,7 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Raises the minimum capacity for new resources given changes to CSC parameters and reinstates the flexibility requirement. Adds HOC hydro opportunity costs into the dispatch for zero marginal cost resources to avoid having to set an artibrary variable OM value for hydro (and corrects that data).
</commit_message>
<xml_diff>
--- a/InputData/elec/CDRDfRCP/Cln Dsptchble Rsrc Dmnd for Rlbty Curve Param.xlsx
+++ b/InputData/elec/CDRDfRCP/Cln Dsptchble Rsrc Dmnd for Rlbty Curve Param.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\CDRDfRCP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Models\US\Models\eps-us\InputData\elec\CDRDfRCP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D7C115-3F36-463E-8E5F-B756F35079A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF19BEF-7B33-4E46-BD1E-8C0B10518330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{DDCF7A3C-4581-48BB-A680-D5CBB461C8EB}"/>
+    <workbookView xWindow="34590" yWindow="45" windowWidth="23010" windowHeight="13770" xr2:uid="{DDCF7A3C-4581-48BB-A680-D5CBB461C8EB}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -503,7 +503,7 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated curve parameters for Clean Dispatchable Supply based on feedback from electricity sector team.
</commit_message>
<xml_diff>
--- a/InputData/elec/CDRDfRCP/Cln Dsptchble Rsrc Dmnd for Rlbty Curve Param.xlsx
+++ b/InputData/elec/CDRDfRCP/Cln Dsptchble Rsrc Dmnd for Rlbty Curve Param.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Models\US\Models\eps-us\InputData\elec\CDRDfRCP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF19BEF-7B33-4E46-BD1E-8C0B10518330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845E5034-0753-4D2F-924A-D8ED6ECB42F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34590" yWindow="45" windowWidth="23010" windowHeight="13770" xr2:uid="{DDCF7A3C-4581-48BB-A680-D5CBB461C8EB}"/>
+    <workbookView xWindow="7080" yWindow="105" windowWidth="29640" windowHeight="21840" xr2:uid="{DDCF7A3C-4581-48BB-A680-D5CBB461C8EB}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>CDRDfRCP Clean Dispatchable Resource Demand for Reliabilty Curve Paramaters</t>
   </si>
@@ -65,12 +65,18 @@
   <si>
     <t>required share peak</t>
   </si>
+  <si>
+    <t>RPS %</t>
+  </si>
+  <si>
+    <t>Required clena firm</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,6 +86,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -104,15 +117,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -125,6 +143,1205 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Percent Clean Firm</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Required at CES Values</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>About!$A$15:$A$63</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.87</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>About!$B$15:$B$63</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>1.3345183610335988E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7757968180565077E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3503723246920407E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0948404411468292E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0548669420009678E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.2871968066592338E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.8620531956736788E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.8659893966219769E-5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1405263483894035E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4609811682472217E-4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.8637901468158136E-4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.3681548265671039E-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.9972778773873499E-4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.7790817418671967E-4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.7470257398569141E-4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.9410250432745957E-4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.4084704568779251E-4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.2053410628561982E-4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.1397391661842615E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.406138252443695E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.7286299009540041E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.1174481702520621E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.5842552420247689E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.1421976435896727E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.8059045878387158E-3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.5914003965626393E-3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5.5158957263671321E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6.5974149898884119E-3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7.8542111497937779E-3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9.3039159295859718E-3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.0962376409663188E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.2842142086152065E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.4950594952808677E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.7287764710475297E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.9843946630412508E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.2597342306981179E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.5512067623070053E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.853699948673204E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.1606027941427882E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.4640289033344603E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.7552809826340114E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.0255641018243658E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.2668969178507668E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.4730964824285228E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.640643664684916E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.7692043118172142E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.8616190328389854E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.9232966777728315E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.9611286513068079E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F525-4D21-B1BB-181E14534A7D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1033414303"/>
+        <c:axId val="1033417663"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1033414303"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1033417663"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1033417663"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1033414303"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9075861-0046-3279-6C90-16C94A6D8E5C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -424,18 +1641,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B207133-CFE8-4DB4-95CD-9BA248AF1C6C}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -443,12 +1663,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -456,13 +1676,463 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>0.52</v>
+      </c>
+      <c r="B15" s="4">
+        <f>(1-EXP(-((A15)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>1.3345183610335988E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="B16" s="4">
+        <f>(1-EXP(-((A16)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>1.7757968180565077E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>0.54</v>
+      </c>
+      <c r="B17" s="4">
+        <f>(1-EXP(-((A17)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>2.3503723246920407E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B18" s="4">
+        <f>(1-EXP(-((A18)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>3.0948404411468292E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="B19" s="4">
+        <f>(1-EXP(-((A19)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>4.0548669420009678E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="B20" s="4">
+        <f>(1-EXP(-((A20)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>5.2871968066592338E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="B21" s="4">
+        <f>(1-EXP(-((A21)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>6.8620531956736788E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>0.59</v>
+      </c>
+      <c r="B22" s="4">
+        <f>(1-EXP(-((A22)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>8.8659893966219769E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="B23" s="4">
+        <f>(1-EXP(-((A23)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>1.1405263483894035E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>0.61</v>
+      </c>
+      <c r="B24" s="4">
+        <f>(1-EXP(-((A24)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>1.4609811682472217E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="B25" s="4">
+        <f>(1-EXP(-((A25)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>1.8637901468158136E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>0.63</v>
+      </c>
+      <c r="B26" s="4">
+        <f>(1-EXP(-((A26)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>2.3681548265671039E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>0.64</v>
+      </c>
+      <c r="B27" s="4">
+        <f>(1-EXP(-((A27)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>2.9972778773873499E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="B28" s="4">
+        <f>(1-EXP(-((A28)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>3.7790817418671967E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>0.66</v>
+      </c>
+      <c r="B29" s="4">
+        <f>(1-EXP(-((A29)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>4.7470257398569141E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>0.67</v>
+      </c>
+      <c r="B30" s="4">
+        <f>(1-EXP(-((A30)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>5.9410250432745957E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>0.68</v>
+      </c>
+      <c r="B31" s="4">
+        <f>(1-EXP(-((A31)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>7.4084704568779251E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>0.69</v>
+      </c>
+      <c r="B32" s="4">
+        <f>(1-EXP(-((A32)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>9.2053410628561982E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="B33" s="4">
+        <f>(1-EXP(-((A33)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>1.1397391661842615E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>0.71</v>
+      </c>
+      <c r="B34" s="4">
+        <f>(1-EXP(-((A34)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>1.406138252443695E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>0.72</v>
+      </c>
+      <c r="B35" s="4">
+        <f>(1-EXP(-((A35)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>1.7286299009540041E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>0.73</v>
+      </c>
+      <c r="B36" s="4">
+        <f>(1-EXP(-((A36)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>2.1174481702520621E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>0.74</v>
+      </c>
+      <c r="B37" s="4">
+        <f>(1-EXP(-((A37)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>2.5842552420247689E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="B38" s="4">
+        <f>(1-EXP(-((A38)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>3.1421976435896727E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>0.76</v>
+      </c>
+      <c r="B39" s="4">
+        <f>(1-EXP(-((A39)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>3.8059045878387158E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>0.77</v>
+      </c>
+      <c r="B40" s="4">
+        <f>(1-EXP(-((A40)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>4.5914003965626393E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="B41" s="4">
+        <f>(1-EXP(-((A41)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>5.5158957263671321E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>0.79</v>
+      </c>
+      <c r="B42" s="4">
+        <f>(1-EXP(-((A42)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>6.5974149898884119E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="B43" s="4">
+        <f>(1-EXP(-((A43)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>7.8542111497937779E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>0.81</v>
+      </c>
+      <c r="B44" s="4">
+        <f>(1-EXP(-((A44)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>9.3039159295859718E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>0.82</v>
+      </c>
+      <c r="B45" s="4">
+        <f>(1-EXP(-((A45)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>1.0962376409663188E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>0.83</v>
+      </c>
+      <c r="B46" s="4">
+        <f>(1-EXP(-((A46)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>1.2842142086152065E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <v>0.84</v>
+      </c>
+      <c r="B47" s="4">
+        <f>(1-EXP(-((A47)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>1.4950594952808677E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="B48" s="4">
+        <f>(1-EXP(-((A48)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>1.7287764710475297E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>0.86</v>
+      </c>
+      <c r="B49" s="4">
+        <f>(1-EXP(-((A49)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>1.9843946630412508E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="B50" s="4">
+        <f>(1-EXP(-((A50)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>2.2597342306981179E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <v>0.88</v>
+      </c>
+      <c r="B51" s="4">
+        <f>(1-EXP(-((A51)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>2.5512067623070053E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="B52" s="4">
+        <f>(1-EXP(-((A52)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>2.853699948673204E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="B53" s="4">
+        <f>(1-EXP(-((A53)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>3.1606027941427882E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="B54" s="4">
+        <f>(1-EXP(-((A54)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>3.4640289033344603E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="3">
+        <v>0.92</v>
+      </c>
+      <c r="B55" s="4">
+        <f>(1-EXP(-((A55)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>3.7552809826340114E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="B56" s="4">
+        <f>(1-EXP(-((A56)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>4.0255641018243658E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
+        <v>0.94</v>
+      </c>
+      <c r="B57" s="4">
+        <f>(1-EXP(-((A57)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>4.2668969178507668E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="B58" s="4">
+        <f>(1-EXP(-((A58)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>4.4730964824285228E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="3">
+        <v>0.96</v>
+      </c>
+      <c r="B59" s="4">
+        <f>(1-EXP(-((A59)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>4.640643664684916E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="3">
+        <v>0.97</v>
+      </c>
+      <c r="B60" s="4">
+        <f>(1-EXP(-((A60)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>4.7692043118172142E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="B61" s="4">
+        <f>(1-EXP(-((A61)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>4.8616190328389854E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="B62" s="4">
+        <f>(1-EXP(-((A62)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>4.9232966777728315E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="3">
+        <v>1</v>
+      </c>
+      <c r="B63" s="4">
+        <f>(1-EXP(-((A63)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
+        <v>4.9611286513068079E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -474,7 +2144,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,7 +2157,7 @@
         <v>7</v>
       </c>
       <c r="B1">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -495,7 +2165,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update CDRDfRCP parameters to not start increasing until ~95% CES
</commit_message>
<xml_diff>
--- a/InputData/elec/CDRDfRCP/Cln Dsptchble Rsrc Dmnd for Rlbty Curve Param.xlsx
+++ b/InputData/elec/CDRDfRCP/Cln Dsptchble Rsrc Dmnd for Rlbty Curve Param.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Models\US\Models\eps-us\InputData\elec\CDRDfRCP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\CDRDfRCP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845E5034-0753-4D2F-924A-D8ED6ECB42F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5650AD1B-C0BA-4B3D-AD2B-DEFFB05BA2A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7080" yWindow="105" windowWidth="29640" windowHeight="21840" xr2:uid="{DDCF7A3C-4581-48BB-A680-D5CBB461C8EB}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{DDCF7A3C-4581-48BB-A680-D5CBB461C8EB}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -403,151 +403,151 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="49"/>
                 <c:pt idx="0">
-                  <c:v>1.3345183610335988E-5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.7757968180565077E-5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.3503723246920407E-5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0948404411468292E-5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0548669420009678E-5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.2871968066592338E-5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.8620531956736788E-5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.8659893966219769E-5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.1405263483894035E-4</c:v>
+                  <c:v>5.551115123125783E-18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.4609811682472217E-4</c:v>
+                  <c:v>1.6653345369377351E-17</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.8637901468158136E-4</c:v>
+                  <c:v>6.1062266354383615E-17</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.3681548265671039E-4</c:v>
+                  <c:v>2.0539125955565397E-16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.9972778773873499E-4</c:v>
+                  <c:v>6.6058269965196816E-16</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.7790817418671967E-4</c:v>
+                  <c:v>2.1149748619109233E-15</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.7470257398569141E-4</c:v>
+                  <c:v>6.6502359175046883E-15</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.9410250432745957E-4</c:v>
+                  <c:v>2.0539125955565396E-14</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7.4084704568779251E-4</c:v>
+                  <c:v>6.2400085099056931E-14</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9.2053410628561982E-4</c:v>
+                  <c:v>1.8650636590678006E-13</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.1397391661842615E-3</c:v>
+                  <c:v>5.4873883215122991E-13</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.406138252443695E-3</c:v>
+                  <c:v>1.5899781491413023E-12</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.7286299009540041E-3</c:v>
+                  <c:v>4.5389081382296588E-12</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.1174481702520621E-3</c:v>
+                  <c:v>1.2771117496868101E-11</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.5842552420247689E-3</c:v>
+                  <c:v>3.5431807487995574E-11</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.1421976435896727E-3</c:v>
+                  <c:v>9.6963675977335131E-11</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.8059045878387158E-3</c:v>
+                  <c:v>2.6183864521023282E-10</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.5914003965626393E-3</c:v>
+                  <c:v>6.9794099943898406E-10</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>5.5158957263671321E-3</c:v>
+                  <c:v>1.8370015453239576E-9</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6.5974149898884119E-3</c:v>
+                  <c:v>4.7758002441611331E-9</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7.8542111497937779E-3</c:v>
+                  <c:v>1.2267704280199966E-8</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>9.3039159295859718E-3</c:v>
+                  <c:v>3.1145162993073687E-8</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.0962376409663188E-2</c:v>
+                  <c:v>7.8172304796009229E-8</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.2842142086152065E-2</c:v>
+                  <c:v>1.9403068323153861E-7</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.4950594952808677E-2</c:v>
+                  <c:v>4.7638569630192865E-7</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.7287764710475297E-2</c:v>
+                  <c:v>1.15725410513301E-6</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.9843946630412508E-2</c:v>
+                  <c:v>2.7821855297760492E-6</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.2597342306981179E-2</c:v>
+                  <c:v>6.6210903952146356E-6</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2.5512067623070053E-2</c:v>
+                  <c:v>1.5600803848198064E-5</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.853699948673204E-2</c:v>
+                  <c:v>3.6400444973472278E-5</c:v>
                 </c:pt>
                 <c:pt idx="38">
+                  <c:v>8.4107941297706379E-5</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.9243394277213E-4</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.3571467423015323E-4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>9.7491479588711078E-4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2.1483338811260355E-3</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.6277060486618286E-3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>9.5923357822252763E-3</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.8541891846878166E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
                   <c:v>3.1606027941427882E-2</c:v>
                 </c:pt>
-                <c:pt idx="39">
-                  <c:v>3.4640289033344603E-2</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>3.7552809826340114E-2</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>4.0255641018243658E-2</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>4.2668969178507668E-2</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>4.4730964824285228E-2</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>4.640643664684916E-2</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>4.7692043118172142E-2</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>4.8616190328389854E-2</c:v>
-                </c:pt>
                 <c:pt idx="47">
-                  <c:v>4.9232966777728315E-2</c:v>
+                  <c:v>4.4125085859779797E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>4.9611286513068079E-2</c:v>
+                  <c:v>4.9471822020543572E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1307,16 +1307,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1644,10 +1644,13 @@
   <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:H1"/>
+      <selection activeCell="K2" sqref="K2:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="20.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1695,7 +1698,7 @@
       </c>
       <c r="B15" s="4">
         <f>(1-EXP(-((A15)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>1.3345183610335988E-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1704,7 +1707,7 @@
       </c>
       <c r="B16" s="4">
         <f>(1-EXP(-((A16)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>1.7757968180565077E-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1713,7 +1716,7 @@
       </c>
       <c r="B17" s="4">
         <f>(1-EXP(-((A17)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>2.3503723246920407E-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1722,7 +1725,7 @@
       </c>
       <c r="B18" s="4">
         <f>(1-EXP(-((A18)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>3.0948404411468292E-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1731,7 +1734,7 @@
       </c>
       <c r="B19" s="4">
         <f>(1-EXP(-((A19)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>4.0548669420009678E-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1740,7 +1743,7 @@
       </c>
       <c r="B20" s="4">
         <f>(1-EXP(-((A20)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>5.2871968066592338E-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1749,7 +1752,7 @@
       </c>
       <c r="B21" s="4">
         <f>(1-EXP(-((A21)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>6.8620531956736788E-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1758,7 +1761,7 @@
       </c>
       <c r="B22" s="4">
         <f>(1-EXP(-((A22)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>8.8659893966219769E-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1767,7 +1770,7 @@
       </c>
       <c r="B23" s="4">
         <f>(1-EXP(-((A23)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>1.1405263483894035E-4</v>
+        <v>5.551115123125783E-18</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1776,7 +1779,7 @@
       </c>
       <c r="B24" s="4">
         <f>(1-EXP(-((A24)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>1.4609811682472217E-4</v>
+        <v>1.6653345369377351E-17</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1785,7 +1788,7 @@
       </c>
       <c r="B25" s="4">
         <f>(1-EXP(-((A25)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>1.8637901468158136E-4</v>
+        <v>6.1062266354383615E-17</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1794,7 +1797,7 @@
       </c>
       <c r="B26" s="4">
         <f>(1-EXP(-((A26)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>2.3681548265671039E-4</v>
+        <v>2.0539125955565397E-16</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1803,7 +1806,7 @@
       </c>
       <c r="B27" s="4">
         <f>(1-EXP(-((A27)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>2.9972778773873499E-4</v>
+        <v>6.6058269965196816E-16</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1812,7 +1815,7 @@
       </c>
       <c r="B28" s="4">
         <f>(1-EXP(-((A28)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>3.7790817418671967E-4</v>
+        <v>2.1149748619109233E-15</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1821,7 +1824,7 @@
       </c>
       <c r="B29" s="4">
         <f>(1-EXP(-((A29)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>4.7470257398569141E-4</v>
+        <v>6.6502359175046883E-15</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1830,7 +1833,7 @@
       </c>
       <c r="B30" s="4">
         <f>(1-EXP(-((A30)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>5.9410250432745957E-4</v>
+        <v>2.0539125955565396E-14</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1839,7 +1842,7 @@
       </c>
       <c r="B31" s="4">
         <f>(1-EXP(-((A31)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>7.4084704568779251E-4</v>
+        <v>6.2400085099056931E-14</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1848,7 +1851,7 @@
       </c>
       <c r="B32" s="4">
         <f>(1-EXP(-((A32)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>9.2053410628561982E-4</v>
+        <v>1.8650636590678006E-13</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1857,7 +1860,7 @@
       </c>
       <c r="B33" s="4">
         <f>(1-EXP(-((A33)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>1.1397391661842615E-3</v>
+        <v>5.4873883215122991E-13</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1866,7 +1869,7 @@
       </c>
       <c r="B34" s="4">
         <f>(1-EXP(-((A34)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>1.406138252443695E-3</v>
+        <v>1.5899781491413023E-12</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1875,7 +1878,7 @@
       </c>
       <c r="B35" s="4">
         <f>(1-EXP(-((A35)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>1.7286299009540041E-3</v>
+        <v>4.5389081382296588E-12</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1884,7 +1887,7 @@
       </c>
       <c r="B36" s="4">
         <f>(1-EXP(-((A36)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>2.1174481702520621E-3</v>
+        <v>1.2771117496868101E-11</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1893,7 +1896,7 @@
       </c>
       <c r="B37" s="4">
         <f>(1-EXP(-((A37)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>2.5842552420247689E-3</v>
+        <v>3.5431807487995574E-11</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1902,7 +1905,7 @@
       </c>
       <c r="B38" s="4">
         <f>(1-EXP(-((A38)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>3.1421976435896727E-3</v>
+        <v>9.6963675977335131E-11</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1911,7 +1914,7 @@
       </c>
       <c r="B39" s="4">
         <f>(1-EXP(-((A39)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>3.8059045878387158E-3</v>
+        <v>2.6183864521023282E-10</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1920,7 +1923,7 @@
       </c>
       <c r="B40" s="4">
         <f>(1-EXP(-((A40)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>4.5914003965626393E-3</v>
+        <v>6.9794099943898406E-10</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1929,7 +1932,7 @@
       </c>
       <c r="B41" s="4">
         <f>(1-EXP(-((A41)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>5.5158957263671321E-3</v>
+        <v>1.8370015453239576E-9</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1938,7 +1941,7 @@
       </c>
       <c r="B42" s="4">
         <f>(1-EXP(-((A42)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>6.5974149898884119E-3</v>
+        <v>4.7758002441611331E-9</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1947,7 +1950,7 @@
       </c>
       <c r="B43" s="4">
         <f>(1-EXP(-((A43)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>7.8542111497937779E-3</v>
+        <v>1.2267704280199966E-8</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -1956,7 +1959,7 @@
       </c>
       <c r="B44" s="4">
         <f>(1-EXP(-((A44)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>9.3039159295859718E-3</v>
+        <v>3.1145162993073687E-8</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1965,7 +1968,7 @@
       </c>
       <c r="B45" s="4">
         <f>(1-EXP(-((A45)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>1.0962376409663188E-2</v>
+        <v>7.8172304796009229E-8</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1974,7 +1977,7 @@
       </c>
       <c r="B46" s="4">
         <f>(1-EXP(-((A46)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>1.2842142086152065E-2</v>
+        <v>1.9403068323153861E-7</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1983,7 +1986,7 @@
       </c>
       <c r="B47" s="4">
         <f>(1-EXP(-((A47)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>1.4950594952808677E-2</v>
+        <v>4.7638569630192865E-7</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1992,7 +1995,7 @@
       </c>
       <c r="B48" s="4">
         <f>(1-EXP(-((A48)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>1.7287764710475297E-2</v>
+        <v>1.15725410513301E-6</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -2001,7 +2004,7 @@
       </c>
       <c r="B49" s="4">
         <f>(1-EXP(-((A49)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>1.9843946630412508E-2</v>
+        <v>2.7821855297760492E-6</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2010,7 +2013,7 @@
       </c>
       <c r="B50" s="4">
         <f>(1-EXP(-((A50)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>2.2597342306981179E-2</v>
+        <v>6.6210903952146356E-6</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2019,7 +2022,7 @@
       </c>
       <c r="B51" s="4">
         <f>(1-EXP(-((A51)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>2.5512067623070053E-2</v>
+        <v>1.5600803848198064E-5</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2028,7 +2031,7 @@
       </c>
       <c r="B52" s="4">
         <f>(1-EXP(-((A52)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>2.853699948673204E-2</v>
+        <v>3.6400444973472278E-5</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -2037,7 +2040,7 @@
       </c>
       <c r="B53" s="4">
         <f>(1-EXP(-((A53)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>3.1606027941427882E-2</v>
+        <v>8.4107941297706379E-5</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -2046,7 +2049,7 @@
       </c>
       <c r="B54" s="4">
         <f>(1-EXP(-((A54)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>3.4640289033344603E-2</v>
+        <v>1.9243394277213E-4</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -2055,7 +2058,7 @@
       </c>
       <c r="B55" s="4">
         <f>(1-EXP(-((A55)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>3.7552809826340114E-2</v>
+        <v>4.3571467423015323E-4</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -2064,7 +2067,7 @@
       </c>
       <c r="B56" s="4">
         <f>(1-EXP(-((A56)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>4.0255641018243658E-2</v>
+        <v>9.7491479588711078E-4</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -2073,7 +2076,7 @@
       </c>
       <c r="B57" s="4">
         <f>(1-EXP(-((A57)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>4.2668969178507668E-2</v>
+        <v>2.1483338811260355E-3</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -2082,7 +2085,7 @@
       </c>
       <c r="B58" s="4">
         <f>(1-EXP(-((A58)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>4.4730964824285228E-2</v>
+        <v>4.6277060486618286E-3</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -2091,7 +2094,7 @@
       </c>
       <c r="B59" s="4">
         <f>(1-EXP(-((A59)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>4.640643664684916E-2</v>
+        <v>9.5923357822252763E-3</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -2100,7 +2103,7 @@
       </c>
       <c r="B60" s="4">
         <f>(1-EXP(-((A60)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>4.7692043118172142E-2</v>
+        <v>1.8541891846878166E-2</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -2109,7 +2112,7 @@
       </c>
       <c r="B61" s="4">
         <f>(1-EXP(-((A61)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>4.8616190328389854E-2</v>
+        <v>3.1606027941427882E-2</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -2118,7 +2121,7 @@
       </c>
       <c r="B62" s="4">
         <f>(1-EXP(-((A62)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>4.9232966777728315E-2</v>
+        <v>4.4125085859779797E-2</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -2127,7 +2130,7 @@
       </c>
       <c r="B63" s="4">
         <f>(1-EXP(-((A63)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>4.9611286513068079E-2</v>
+        <v>4.9471822020543572E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2144,7 +2147,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2157,7 +2160,7 @@
         <v>7</v>
       </c>
       <c r="B1">
-        <v>15</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2165,7 +2168,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>0.9</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Revert CDRDfRCP parameters to avoid artificially high CES credit prices
</commit_message>
<xml_diff>
--- a/InputData/elec/CDRDfRCP/Cln Dsptchble Rsrc Dmnd for Rlbty Curve Param.xlsx
+++ b/InputData/elec/CDRDfRCP/Cln Dsptchble Rsrc Dmnd for Rlbty Curve Param.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\CDRDfRCP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5650AD1B-C0BA-4B3D-AD2B-DEFFB05BA2A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5881D2B-FBBE-4E3A-97DC-892210235A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{DDCF7A3C-4581-48BB-A680-D5CBB461C8EB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{DDCF7A3C-4581-48BB-A680-D5CBB461C8EB}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>CDRDfRCP Clean Dispatchable Resource Demand for Reliabilty Curve Paramaters</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Required clena firm</t>
+  </si>
+  <si>
+    <t>We avoid having this increase too sharply in the last few percent of requirement to avoid</t>
+  </si>
+  <si>
+    <t>artificially high CES credit prices in the model.</t>
   </si>
 </sst>
 </file>
@@ -403,151 +409,151 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="49"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1.3345183610335988E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1.7757968180565077E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2.3503723246920407E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>3.0948404411468292E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>4.0548669420009678E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>5.2871968066592338E-5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>6.8620531956736788E-5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>8.8659893966219769E-5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.551115123125783E-18</c:v>
+                  <c:v>1.1405263483894035E-4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.6653345369377351E-17</c:v>
+                  <c:v>1.4609811682472217E-4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.1062266354383615E-17</c:v>
+                  <c:v>1.8637901468158136E-4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.0539125955565397E-16</c:v>
+                  <c:v>2.3681548265671039E-4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.6058269965196816E-16</c:v>
+                  <c:v>2.9972778773873499E-4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.1149748619109233E-15</c:v>
+                  <c:v>3.7790817418671967E-4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.6502359175046883E-15</c:v>
+                  <c:v>4.7470257398569141E-4</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.0539125955565396E-14</c:v>
+                  <c:v>5.9410250432745957E-4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.2400085099056931E-14</c:v>
+                  <c:v>7.4084704568779251E-4</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.8650636590678006E-13</c:v>
+                  <c:v>9.2053410628561982E-4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.4873883215122991E-13</c:v>
+                  <c:v>1.1397391661842615E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.5899781491413023E-12</c:v>
+                  <c:v>1.406138252443695E-3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.5389081382296588E-12</c:v>
+                  <c:v>1.7286299009540041E-3</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.2771117496868101E-11</c:v>
+                  <c:v>2.1174481702520621E-3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.5431807487995574E-11</c:v>
+                  <c:v>2.5842552420247689E-3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9.6963675977335131E-11</c:v>
+                  <c:v>3.1421976435896727E-3</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.6183864521023282E-10</c:v>
+                  <c:v>3.8059045878387158E-3</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>6.9794099943898406E-10</c:v>
+                  <c:v>4.5914003965626393E-3</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.8370015453239576E-9</c:v>
+                  <c:v>5.5158957263671321E-3</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.7758002441611331E-9</c:v>
+                  <c:v>6.5974149898884119E-3</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.2267704280199966E-8</c:v>
+                  <c:v>7.8542111497937779E-3</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.1145162993073687E-8</c:v>
+                  <c:v>9.3039159295859718E-3</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>7.8172304796009229E-8</c:v>
+                  <c:v>1.0962376409663188E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.9403068323153861E-7</c:v>
+                  <c:v>1.2842142086152065E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.7638569630192865E-7</c:v>
+                  <c:v>1.4950594952808677E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.15725410513301E-6</c:v>
+                  <c:v>1.7287764710475297E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.7821855297760492E-6</c:v>
+                  <c:v>1.9843946630412508E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>6.6210903952146356E-6</c:v>
+                  <c:v>2.2597342306981179E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.5600803848198064E-5</c:v>
+                  <c:v>2.5512067623070053E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>3.6400444973472278E-5</c:v>
+                  <c:v>2.853699948673204E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>8.4107941297706379E-5</c:v>
+                  <c:v>3.1606027941427882E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1.9243394277213E-4</c:v>
+                  <c:v>3.4640289033344603E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4.3571467423015323E-4</c:v>
+                  <c:v>3.7552809826340114E-2</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>9.7491479588711078E-4</c:v>
+                  <c:v>4.0255641018243658E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2.1483338811260355E-3</c:v>
+                  <c:v>4.2668969178507668E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4.6277060486618286E-3</c:v>
+                  <c:v>4.4730964824285228E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>9.5923357822252763E-3</c:v>
+                  <c:v>4.640643664684916E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1.8541891846878166E-2</c:v>
+                  <c:v>4.7692043118172142E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>3.1606027941427882E-2</c:v>
+                  <c:v>4.8616190328389854E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4.4125085859779797E-2</c:v>
+                  <c:v>4.9232966777728315E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>4.9471822020543572E-2</c:v>
+                  <c:v>4.9611286513068079E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1644,7 +1650,7 @@
   <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:L4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1684,6 +1690,16 @@
         <v>6</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
@@ -1698,7 +1714,7 @@
       </c>
       <c r="B15" s="4">
         <f>(1-EXP(-((A15)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>0</v>
+        <v>1.3345183610335988E-5</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1707,7 +1723,7 @@
       </c>
       <c r="B16" s="4">
         <f>(1-EXP(-((A16)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>0</v>
+        <v>1.7757968180565077E-5</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1716,7 +1732,7 @@
       </c>
       <c r="B17" s="4">
         <f>(1-EXP(-((A17)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>0</v>
+        <v>2.3503723246920407E-5</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1725,7 +1741,7 @@
       </c>
       <c r="B18" s="4">
         <f>(1-EXP(-((A18)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>0</v>
+        <v>3.0948404411468292E-5</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1734,7 +1750,7 @@
       </c>
       <c r="B19" s="4">
         <f>(1-EXP(-((A19)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>0</v>
+        <v>4.0548669420009678E-5</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1743,7 +1759,7 @@
       </c>
       <c r="B20" s="4">
         <f>(1-EXP(-((A20)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>0</v>
+        <v>5.2871968066592338E-5</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1752,7 +1768,7 @@
       </c>
       <c r="B21" s="4">
         <f>(1-EXP(-((A21)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>0</v>
+        <v>6.8620531956736788E-5</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1761,7 +1777,7 @@
       </c>
       <c r="B22" s="4">
         <f>(1-EXP(-((A22)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>0</v>
+        <v>8.8659893966219769E-5</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1770,7 +1786,7 @@
       </c>
       <c r="B23" s="4">
         <f>(1-EXP(-((A23)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>5.551115123125783E-18</v>
+        <v>1.1405263483894035E-4</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1779,7 +1795,7 @@
       </c>
       <c r="B24" s="4">
         <f>(1-EXP(-((A24)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>1.6653345369377351E-17</v>
+        <v>1.4609811682472217E-4</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1788,7 +1804,7 @@
       </c>
       <c r="B25" s="4">
         <f>(1-EXP(-((A25)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>6.1062266354383615E-17</v>
+        <v>1.8637901468158136E-4</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1797,7 +1813,7 @@
       </c>
       <c r="B26" s="4">
         <f>(1-EXP(-((A26)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>2.0539125955565397E-16</v>
+        <v>2.3681548265671039E-4</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1806,7 +1822,7 @@
       </c>
       <c r="B27" s="4">
         <f>(1-EXP(-((A27)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>6.6058269965196816E-16</v>
+        <v>2.9972778773873499E-4</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1815,7 +1831,7 @@
       </c>
       <c r="B28" s="4">
         <f>(1-EXP(-((A28)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>2.1149748619109233E-15</v>
+        <v>3.7790817418671967E-4</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1824,7 +1840,7 @@
       </c>
       <c r="B29" s="4">
         <f>(1-EXP(-((A29)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>6.6502359175046883E-15</v>
+        <v>4.7470257398569141E-4</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1833,7 +1849,7 @@
       </c>
       <c r="B30" s="4">
         <f>(1-EXP(-((A30)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>2.0539125955565396E-14</v>
+        <v>5.9410250432745957E-4</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1842,7 +1858,7 @@
       </c>
       <c r="B31" s="4">
         <f>(1-EXP(-((A31)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>6.2400085099056931E-14</v>
+        <v>7.4084704568779251E-4</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1851,7 +1867,7 @@
       </c>
       <c r="B32" s="4">
         <f>(1-EXP(-((A32)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>1.8650636590678006E-13</v>
+        <v>9.2053410628561982E-4</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1860,7 +1876,7 @@
       </c>
       <c r="B33" s="4">
         <f>(1-EXP(-((A33)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>5.4873883215122991E-13</v>
+        <v>1.1397391661842615E-3</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1869,7 +1885,7 @@
       </c>
       <c r="B34" s="4">
         <f>(1-EXP(-((A34)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>1.5899781491413023E-12</v>
+        <v>1.406138252443695E-3</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1878,7 +1894,7 @@
       </c>
       <c r="B35" s="4">
         <f>(1-EXP(-((A35)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>4.5389081382296588E-12</v>
+        <v>1.7286299009540041E-3</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1887,7 +1903,7 @@
       </c>
       <c r="B36" s="4">
         <f>(1-EXP(-((A36)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>1.2771117496868101E-11</v>
+        <v>2.1174481702520621E-3</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1896,7 +1912,7 @@
       </c>
       <c r="B37" s="4">
         <f>(1-EXP(-((A37)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>3.5431807487995574E-11</v>
+        <v>2.5842552420247689E-3</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1905,7 +1921,7 @@
       </c>
       <c r="B38" s="4">
         <f>(1-EXP(-((A38)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>9.6963675977335131E-11</v>
+        <v>3.1421976435896727E-3</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1914,7 +1930,7 @@
       </c>
       <c r="B39" s="4">
         <f>(1-EXP(-((A39)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>2.6183864521023282E-10</v>
+        <v>3.8059045878387158E-3</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1923,7 +1939,7 @@
       </c>
       <c r="B40" s="4">
         <f>(1-EXP(-((A40)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>6.9794099943898406E-10</v>
+        <v>4.5914003965626393E-3</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1932,7 +1948,7 @@
       </c>
       <c r="B41" s="4">
         <f>(1-EXP(-((A41)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>1.8370015453239576E-9</v>
+        <v>5.5158957263671321E-3</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1941,7 +1957,7 @@
       </c>
       <c r="B42" s="4">
         <f>(1-EXP(-((A42)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>4.7758002441611331E-9</v>
+        <v>6.5974149898884119E-3</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1950,7 +1966,7 @@
       </c>
       <c r="B43" s="4">
         <f>(1-EXP(-((A43)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>1.2267704280199966E-8</v>
+        <v>7.8542111497937779E-3</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -1959,7 +1975,7 @@
       </c>
       <c r="B44" s="4">
         <f>(1-EXP(-((A44)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>3.1145162993073687E-8</v>
+        <v>9.3039159295859718E-3</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1968,7 +1984,7 @@
       </c>
       <c r="B45" s="4">
         <f>(1-EXP(-((A45)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>7.8172304796009229E-8</v>
+        <v>1.0962376409663188E-2</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1977,7 +1993,7 @@
       </c>
       <c r="B46" s="4">
         <f>(1-EXP(-((A46)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>1.9403068323153861E-7</v>
+        <v>1.2842142086152065E-2</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1986,7 +2002,7 @@
       </c>
       <c r="B47" s="4">
         <f>(1-EXP(-((A47)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>4.7638569630192865E-7</v>
+        <v>1.4950594952808677E-2</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1995,7 +2011,7 @@
       </c>
       <c r="B48" s="4">
         <f>(1-EXP(-((A48)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>1.15725410513301E-6</v>
+        <v>1.7287764710475297E-2</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -2004,7 +2020,7 @@
       </c>
       <c r="B49" s="4">
         <f>(1-EXP(-((A49)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>2.7821855297760492E-6</v>
+        <v>1.9843946630412508E-2</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2013,7 +2029,7 @@
       </c>
       <c r="B50" s="4">
         <f>(1-EXP(-((A50)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>6.6210903952146356E-6</v>
+        <v>2.2597342306981179E-2</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2022,7 +2038,7 @@
       </c>
       <c r="B51" s="4">
         <f>(1-EXP(-((A51)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>1.5600803848198064E-5</v>
+        <v>2.5512067623070053E-2</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2031,7 +2047,7 @@
       </c>
       <c r="B52" s="4">
         <f>(1-EXP(-((A52)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>3.6400444973472278E-5</v>
+        <v>2.853699948673204E-2</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -2040,7 +2056,7 @@
       </c>
       <c r="B53" s="4">
         <f>(1-EXP(-((A53)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>8.4107941297706379E-5</v>
+        <v>3.1606027941427882E-2</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -2049,7 +2065,7 @@
       </c>
       <c r="B54" s="4">
         <f>(1-EXP(-((A54)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>1.9243394277213E-4</v>
+        <v>3.4640289033344603E-2</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -2058,7 +2074,7 @@
       </c>
       <c r="B55" s="4">
         <f>(1-EXP(-((A55)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>4.3571467423015323E-4</v>
+        <v>3.7552809826340114E-2</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -2067,7 +2083,7 @@
       </c>
       <c r="B56" s="4">
         <f>(1-EXP(-((A56)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>9.7491479588711078E-4</v>
+        <v>4.0255641018243658E-2</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -2076,7 +2092,7 @@
       </c>
       <c r="B57" s="4">
         <f>(1-EXP(-((A57)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>2.1483338811260355E-3</v>
+        <v>4.2668969178507668E-2</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -2085,7 +2101,7 @@
       </c>
       <c r="B58" s="4">
         <f>(1-EXP(-((A58)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>4.6277060486618286E-3</v>
+        <v>4.4730964824285228E-2</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -2094,7 +2110,7 @@
       </c>
       <c r="B59" s="4">
         <f>(1-EXP(-((A59)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>9.5923357822252763E-3</v>
+        <v>4.640643664684916E-2</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -2103,7 +2119,7 @@
       </c>
       <c r="B60" s="4">
         <f>(1-EXP(-((A60)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>1.8541891846878166E-2</v>
+        <v>4.7692043118172142E-2</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -2112,7 +2128,7 @@
       </c>
       <c r="B61" s="4">
         <f>(1-EXP(-((A61)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>3.1606027941427882E-2</v>
+        <v>4.8616190328389854E-2</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -2121,7 +2137,7 @@
       </c>
       <c r="B62" s="4">
         <f>(1-EXP(-((A62)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>4.4125085859779797E-2</v>
+        <v>4.9232966777728315E-2</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -2130,7 +2146,7 @@
       </c>
       <c r="B63" s="4">
         <f>(1-EXP(-((A63)/CDRDfRCP!$B$2)^CDRDfRCP!$B$1))*CDRDfRCP!$B$3</f>
-        <v>4.9471822020543572E-2</v>
+        <v>4.9611286513068079E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2147,7 +2163,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2160,7 +2176,7 @@
         <v>7</v>
       </c>
       <c r="B1">
-        <v>75</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2168,7 +2184,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>0.98</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>